<commit_message>
Refactor code formatting and remove unnecessary imports
</commit_message>
<xml_diff>
--- a/Статистика.xlsx
+++ b/Статистика.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="54">
   <si>
     <t>ID в Телеграм</t>
   </si>
@@ -162,10 +162,22 @@
     <t>21.08.2024 12:21:23</t>
   </si>
   <si>
+    <t>21.08.2024 16:38:46</t>
+  </si>
+  <si>
+    <t>21.08.2024 16:39:08</t>
+  </si>
+  <si>
+    <t>21.08.2024 16:39:47</t>
+  </si>
+  <si>
     <t>20.08.2024 22:39:18</t>
   </si>
   <si>
     <t>21.08.2024 12:21:25</t>
+  </si>
+  <si>
+    <t>21.08.2024 16:39:12</t>
   </si>
 </sst>
 </file>
@@ -639,13 +651,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
@@ -917,6 +929,48 @@
         <v>47</v>
       </c>
     </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -924,15 +978,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -961,7 +1015,7 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -975,7 +1029,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -989,7 +1043,35 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>